<commit_message>
add data array curve
</commit_message>
<xml_diff>
--- a/server/pattern/Pattern.xlsx
+++ b/server/pattern/Pattern.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wi-backend\server\pattern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\wi-backend\server\pattern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A67C033-48B3-44F2-8D60-72CD86C3EEA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974E7AA9-A8B8-44B2-8180-EDE461A05DC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -880,9 +880,6 @@
     <t>Typical</t>
   </si>
   <si>
-    <t>Uniform_grain size</t>
-  </si>
-  <si>
     <t>Coarsening_upward</t>
   </si>
   <si>
@@ -896,6 +893,9 @@
   </si>
   <si>
     <t>Uniform grain size</t>
+  </si>
+  <si>
+    <t>Uniform_grain_size</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1299,7 @@
   <dimension ref="A1:Y993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2070,10 +2070,10 @@
     </row>
     <row r="24" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C24" s="9">
         <v>23</v>
@@ -2103,10 +2103,10 @@
     </row>
     <row r="25" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C25" s="9">
         <v>24</v>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="26" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C26" s="9">
         <v>25</v>

</xml_diff>